<commit_message>
updated lab1 by teachers comments
</commit_message>
<xml_diff>
--- a/lab1-14.02.21/codes_diagrams.xlsx
+++ b/lab1-14.02.21/codes_diagrams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\itmo\3 course\computer networks\lab1-14.02.21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF34F18-3C7C-4AE6-8536-18459E909CE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70B0553-7679-42CE-A0AC-308809CDB170}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>NRZ</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>скремблирование (Bi = Ai⊕Bi-3⊕Bi-5))</t>
+  </si>
+  <si>
+    <t>Манчестреский</t>
+  </si>
+  <si>
+    <t>Манчестерский</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL53"/>
+  <dimension ref="A1:BL63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BN43" sqref="BN43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,519 +1878,822 @@
       <c r="AV42" s="3"/>
       <c r="AW42" s="3"/>
     </row>
-    <row r="44" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+    <row r="43" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="I43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="V43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AN43" s="15"/>
+      <c r="AP43" s="1"/>
+      <c r="AR43" s="1"/>
+      <c r="AZ43" s="1"/>
+      <c r="BA43" s="1"/>
+      <c r="BB43" s="15"/>
+    </row>
+    <row r="44" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="13"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="12"/>
+      <c r="AD44" s="10"/>
+      <c r="AE44" s="13"/>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="15"/>
+      <c r="AI44" s="12"/>
+      <c r="AJ44" s="5"/>
+      <c r="AK44" s="7"/>
+      <c r="AL44" s="15"/>
+      <c r="AM44" s="12"/>
+      <c r="AN44" s="10"/>
+      <c r="AO44" s="13"/>
+      <c r="AP44" s="10"/>
+      <c r="AQ44" s="13"/>
+      <c r="AR44" s="10"/>
+      <c r="AS44" s="13"/>
+      <c r="AT44" s="5"/>
+      <c r="AU44" s="7"/>
+      <c r="AV44" s="13"/>
+      <c r="AW44" s="5"/>
+      <c r="AX44" s="2"/>
+      <c r="AY44" s="12"/>
+      <c r="AZ44" s="15"/>
+      <c r="BA44" s="7"/>
+      <c r="BB44" s="15"/>
+      <c r="BC44" s="12"/>
+      <c r="BD44" s="10"/>
+      <c r="BE44" s="13"/>
+      <c r="BF44" s="10"/>
+      <c r="BG44" s="13"/>
+      <c r="BH44" s="10"/>
+      <c r="BI44" s="13"/>
+      <c r="BJ44" s="10"/>
+      <c r="BK44" s="13"/>
+      <c r="BL44" s="5"/>
+    </row>
+    <row r="45" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="9"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="9"/>
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="6"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="9"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="12"/>
+      <c r="AH45" s="6"/>
+      <c r="AI45" s="4"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="12"/>
+      <c r="AL45" s="6"/>
+      <c r="AM45" s="4"/>
+      <c r="AN45" s="13"/>
+      <c r="AO45" s="9"/>
+      <c r="AP45" s="13"/>
+      <c r="AQ45" s="9"/>
+      <c r="AR45" s="13"/>
+      <c r="AS45" s="9"/>
+      <c r="AT45" s="15"/>
+      <c r="AU45" s="12"/>
+      <c r="AV45" s="9"/>
+      <c r="AW45" s="15"/>
+      <c r="AX45" s="6"/>
+      <c r="AY45" s="4"/>
+      <c r="AZ45" s="15"/>
+      <c r="BA45" s="12"/>
+      <c r="BB45" s="6"/>
+      <c r="BC45" s="4"/>
+      <c r="BD45" s="13"/>
+      <c r="BE45" s="9"/>
+      <c r="BF45" s="13"/>
+      <c r="BG45" s="9"/>
+      <c r="BH45" s="13"/>
+      <c r="BI45" s="9"/>
+      <c r="BJ45" s="15"/>
+      <c r="BK45" s="9"/>
+      <c r="BL45" s="15"/>
+    </row>
+    <row r="46" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3"/>
+      <c r="C46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="Q46" s="3"/>
+      <c r="S46" s="15"/>
+      <c r="AM46" s="15"/>
+      <c r="AR46" s="15"/>
+      <c r="AT46" s="15"/>
+      <c r="AV46" s="3"/>
+      <c r="BC46" s="3"/>
+      <c r="BE46" s="3"/>
+      <c r="BG46" s="15"/>
+      <c r="BJ46" s="15"/>
+      <c r="BK46" s="3"/>
+      <c r="BL46" s="15"/>
+    </row>
+    <row r="47" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="K47" s="15"/>
+    </row>
+    <row r="50" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="18"/>
-      <c r="AA44" s="18"/>
-      <c r="AB44" s="18"/>
-      <c r="AC44" s="18"/>
-      <c r="AD44" s="18"/>
-      <c r="AE44" s="18"/>
-      <c r="AF44" s="18"/>
-      <c r="AG44" s="18"/>
-      <c r="AH44" s="18"/>
-      <c r="AI44" s="18"/>
-      <c r="AJ44" s="18"/>
-      <c r="AK44" s="18"/>
-      <c r="AL44" s="18"/>
-      <c r="AM44" s="18"/>
-      <c r="AN44" s="18"/>
-      <c r="AO44" s="18"/>
-      <c r="AP44" s="18"/>
-      <c r="AQ44" s="18"/>
-      <c r="AR44" s="18"/>
-      <c r="AS44" s="18"/>
-      <c r="AT44" s="18"/>
-      <c r="AU44" s="18"/>
-      <c r="AV44" s="18"/>
-      <c r="AW44" s="18"/>
-      <c r="AX44" s="18"/>
-      <c r="AY44" s="18"/>
-      <c r="AZ44" s="18"/>
-      <c r="BA44" s="18"/>
-      <c r="BB44" s="18"/>
-      <c r="BC44" s="18"/>
-      <c r="BD44" s="18"/>
-      <c r="BE44" s="18"/>
-      <c r="BF44" s="18"/>
-      <c r="BG44" s="18"/>
-      <c r="BH44" s="18"/>
-      <c r="BI44" s="18"/>
-      <c r="BJ44" s="18"/>
-      <c r="BK44" s="18"/>
-      <c r="BL44" s="18"/>
-    </row>
-    <row r="45" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A45" s="17">
-        <v>1</v>
-      </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17">
-        <v>1</v>
-      </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17">
-        <v>0</v>
-      </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17">
-        <v>1</v>
-      </c>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17">
-        <v>0</v>
-      </c>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17">
-        <v>1</v>
-      </c>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17">
-        <v>0</v>
-      </c>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17">
-        <v>1</v>
-      </c>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17">
-        <v>1</v>
-      </c>
-      <c r="R45" s="17"/>
-      <c r="S45" s="17">
-        <v>1</v>
-      </c>
-      <c r="T45" s="17"/>
-      <c r="U45" s="17">
-        <v>1</v>
-      </c>
-      <c r="V45" s="17"/>
-      <c r="W45" s="17">
-        <v>1</v>
-      </c>
-      <c r="X45" s="17"/>
-      <c r="Y45" s="17">
-        <v>1</v>
-      </c>
-      <c r="Z45" s="17"/>
-      <c r="AA45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="17"/>
-      <c r="AC45" s="17">
-        <v>1</v>
-      </c>
-      <c r="AD45" s="17"/>
-      <c r="AE45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="17"/>
-      <c r="AG45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH45" s="17"/>
-      <c r="AI45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL45" s="17"/>
-      <c r="AM45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AN45" s="17"/>
-      <c r="AO45" s="17">
-        <v>1</v>
-      </c>
-      <c r="AP45" s="17"/>
-      <c r="AQ45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR45" s="17"/>
-      <c r="AS45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT45" s="17"/>
-      <c r="AU45" s="17">
-        <v>1</v>
-      </c>
-      <c r="AV45" s="17"/>
-      <c r="AW45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AX45" s="17"/>
-      <c r="AY45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ45" s="17"/>
-      <c r="BA45" s="17">
-        <v>1</v>
-      </c>
-      <c r="BB45" s="17"/>
-      <c r="BC45" s="17">
-        <v>1</v>
-      </c>
-      <c r="BD45" s="17"/>
-      <c r="BE45" s="17">
-        <v>1</v>
-      </c>
-      <c r="BF45" s="17"/>
-      <c r="BG45" s="17">
-        <v>0</v>
-      </c>
-      <c r="BH45" s="17"/>
-      <c r="BI45" s="17">
-        <v>1</v>
-      </c>
-      <c r="BJ45" s="17"/>
-      <c r="BK45" s="17">
-        <v>1</v>
-      </c>
-      <c r="BL45" s="17"/>
-    </row>
-    <row r="46" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+      <c r="V50" s="18"/>
+      <c r="W50" s="18"/>
+      <c r="X50" s="18"/>
+      <c r="Y50" s="18"/>
+      <c r="Z50" s="18"/>
+      <c r="AA50" s="18"/>
+      <c r="AB50" s="18"/>
+      <c r="AC50" s="18"/>
+      <c r="AD50" s="18"/>
+      <c r="AE50" s="18"/>
+      <c r="AF50" s="18"/>
+      <c r="AG50" s="18"/>
+      <c r="AH50" s="18"/>
+      <c r="AI50" s="18"/>
+      <c r="AJ50" s="18"/>
+      <c r="AK50" s="18"/>
+      <c r="AL50" s="18"/>
+      <c r="AM50" s="18"/>
+      <c r="AN50" s="18"/>
+      <c r="AO50" s="18"/>
+      <c r="AP50" s="18"/>
+      <c r="AQ50" s="18"/>
+      <c r="AR50" s="18"/>
+      <c r="AS50" s="18"/>
+      <c r="AT50" s="18"/>
+      <c r="AU50" s="18"/>
+      <c r="AV50" s="18"/>
+      <c r="AW50" s="18"/>
+      <c r="AX50" s="18"/>
+      <c r="AY50" s="18"/>
+      <c r="AZ50" s="18"/>
+      <c r="BA50" s="18"/>
+      <c r="BB50" s="18"/>
+      <c r="BC50" s="18"/>
+      <c r="BD50" s="18"/>
+      <c r="BE50" s="18"/>
+      <c r="BF50" s="18"/>
+      <c r="BG50" s="18"/>
+      <c r="BH50" s="18"/>
+      <c r="BI50" s="18"/>
+      <c r="BJ50" s="18"/>
+      <c r="BK50" s="18"/>
+      <c r="BL50" s="18"/>
+    </row>
+    <row r="51" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A51" s="17">
+        <v>1</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17">
+        <v>1</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17">
+        <v>0</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17">
+        <v>1</v>
+      </c>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17">
+        <v>0</v>
+      </c>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17">
+        <v>1</v>
+      </c>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17">
+        <v>0</v>
+      </c>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17">
+        <v>1</v>
+      </c>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17">
+        <v>1</v>
+      </c>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17">
+        <v>1</v>
+      </c>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17">
+        <v>1</v>
+      </c>
+      <c r="V51" s="17"/>
+      <c r="W51" s="17">
+        <v>1</v>
+      </c>
+      <c r="X51" s="17"/>
+      <c r="Y51" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="17"/>
+      <c r="AA51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="17"/>
+      <c r="AC51" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD51" s="17"/>
+      <c r="AE51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="17"/>
+      <c r="AG51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="17"/>
+      <c r="AI51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="17"/>
+      <c r="AK51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="17"/>
+      <c r="AM51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AN51" s="17"/>
+      <c r="AO51" s="17">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="17"/>
+      <c r="AQ51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR51" s="17"/>
+      <c r="AS51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AT51" s="17"/>
+      <c r="AU51" s="17">
+        <v>1</v>
+      </c>
+      <c r="AV51" s="17"/>
+      <c r="AW51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX51" s="17"/>
+      <c r="AY51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ51" s="17"/>
+      <c r="BA51" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB51" s="17"/>
+      <c r="BC51" s="17">
+        <v>1</v>
+      </c>
+      <c r="BD51" s="17"/>
+      <c r="BE51" s="17">
+        <v>1</v>
+      </c>
+      <c r="BF51" s="17"/>
+      <c r="BG51" s="17">
+        <v>0</v>
+      </c>
+      <c r="BH51" s="17"/>
+      <c r="BI51" s="17">
+        <v>1</v>
+      </c>
+      <c r="BJ51" s="17"/>
+      <c r="BK51" s="17">
+        <v>1</v>
+      </c>
+      <c r="BL51" s="17"/>
+    </row>
+    <row r="52" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="1"/>
-      <c r="AF46" s="15"/>
-      <c r="AX46" s="15"/>
-      <c r="AY46" s="15"/>
-      <c r="BA46" s="15"/>
-      <c r="BD46" s="1"/>
-      <c r="BF46" s="15"/>
-      <c r="BJ46" s="15"/>
-    </row>
-    <row r="47" spans="1:64" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="12"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="7"/>
-      <c r="Y47" s="15"/>
-      <c r="Z47" s="15"/>
-      <c r="AA47" s="15"/>
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="7"/>
-      <c r="AE47" s="6"/>
-      <c r="AF47" s="1"/>
-      <c r="AG47" s="15"/>
-      <c r="AH47" s="15"/>
-      <c r="AI47" s="15"/>
-      <c r="AJ47" s="1"/>
-      <c r="AK47" s="1"/>
-      <c r="AL47" s="15"/>
-      <c r="AM47" s="15"/>
-      <c r="AN47" s="15"/>
-      <c r="AO47" s="15"/>
-      <c r="AP47" s="15"/>
-      <c r="AQ47" s="15"/>
-      <c r="AR47" s="1"/>
-      <c r="AS47" s="1"/>
-      <c r="AT47" s="1"/>
-      <c r="AU47" s="5"/>
-      <c r="AV47" s="3"/>
-      <c r="AW47" s="6"/>
-      <c r="AX47" s="15"/>
-      <c r="AY47" s="1"/>
-      <c r="AZ47" s="1"/>
-      <c r="BA47" s="15"/>
-      <c r="BB47" s="15"/>
-      <c r="BC47" s="5"/>
-      <c r="BD47" s="7"/>
-      <c r="BE47" s="15"/>
-      <c r="BF47" s="15"/>
-      <c r="BG47" s="1"/>
-      <c r="BH47" s="1"/>
-      <c r="BI47" s="5"/>
-      <c r="BJ47" s="7"/>
-      <c r="BK47" s="15"/>
-      <c r="BL47" s="15"/>
-    </row>
-    <row r="48" spans="1:64" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="6"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="12"/>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="1"/>
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="3"/>
-      <c r="AC48" s="15"/>
-      <c r="AD48" s="15"/>
-      <c r="AE48" s="15"/>
-      <c r="AF48" s="15"/>
-      <c r="AG48" s="3"/>
-      <c r="AH48" s="3"/>
-      <c r="AI48" s="3"/>
-      <c r="AJ48" s="15"/>
-      <c r="AK48" s="15"/>
-      <c r="AL48" s="3"/>
-      <c r="AM48" s="3"/>
-      <c r="AN48" s="7"/>
-      <c r="AO48" s="6"/>
-      <c r="AP48" s="1"/>
-      <c r="AQ48" s="5"/>
-      <c r="AR48" s="15"/>
-      <c r="AS48" s="15"/>
-      <c r="AT48" s="15"/>
-      <c r="AU48" s="15"/>
-      <c r="AV48" s="15"/>
-      <c r="AW48" s="15"/>
-      <c r="AX48" s="3"/>
-      <c r="AY48" s="15"/>
-      <c r="AZ48" s="15"/>
-      <c r="BA48" s="6"/>
-      <c r="BB48" s="1"/>
-      <c r="BC48" s="2"/>
-      <c r="BD48" s="12"/>
-      <c r="BE48" s="15"/>
-      <c r="BF48" s="1"/>
-      <c r="BG48" s="2"/>
-      <c r="BH48" s="15"/>
-      <c r="BI48" s="15"/>
-      <c r="BJ48" s="15"/>
-      <c r="BK48" s="2"/>
-      <c r="BL48" s="15"/>
-    </row>
-    <row r="49" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="AA49" s="15"/>
-      <c r="AG49" s="15"/>
-      <c r="AH49" s="15"/>
-      <c r="AK49" s="15"/>
-      <c r="AS49" s="15"/>
-      <c r="AW49" s="15"/>
-      <c r="AY49" s="15"/>
-      <c r="BB49" s="15"/>
-      <c r="BE49" s="3"/>
-      <c r="BI49" s="15"/>
-      <c r="BK49" s="3"/>
-      <c r="BL49" s="3"/>
-    </row>
-    <row r="50" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="B52" s="1"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="1"/>
+      <c r="AF52" s="15"/>
+      <c r="AX52" s="15"/>
+      <c r="AY52" s="15"/>
+      <c r="BA52" s="15"/>
+      <c r="BD52" s="1"/>
+      <c r="BF52" s="15"/>
+      <c r="BJ52" s="15"/>
+    </row>
+    <row r="53" spans="1:64" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="2"/>
+      <c r="V53" s="12"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="15"/>
+      <c r="Z53" s="15"/>
+      <c r="AA53" s="15"/>
+      <c r="AB53" s="15"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="6"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="15"/>
+      <c r="AH53" s="15"/>
+      <c r="AI53" s="15"/>
+      <c r="AJ53" s="1"/>
+      <c r="AK53" s="1"/>
+      <c r="AL53" s="15"/>
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="15"/>
+      <c r="AO53" s="15"/>
+      <c r="AP53" s="15"/>
+      <c r="AQ53" s="15"/>
+      <c r="AR53" s="1"/>
+      <c r="AS53" s="1"/>
+      <c r="AT53" s="1"/>
+      <c r="AU53" s="5"/>
+      <c r="AV53" s="3"/>
+      <c r="AW53" s="6"/>
+      <c r="AX53" s="15"/>
+      <c r="AY53" s="1"/>
+      <c r="AZ53" s="1"/>
+      <c r="BA53" s="15"/>
+      <c r="BB53" s="15"/>
+      <c r="BC53" s="5"/>
+      <c r="BD53" s="7"/>
+      <c r="BE53" s="15"/>
+      <c r="BF53" s="15"/>
+      <c r="BG53" s="1"/>
+      <c r="BH53" s="1"/>
+      <c r="BI53" s="5"/>
+      <c r="BJ53" s="7"/>
+      <c r="BK53" s="15"/>
+      <c r="BL53" s="15"/>
+    </row>
+    <row r="54" spans="1:64" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="12"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="3"/>
+      <c r="AC54" s="15"/>
+      <c r="AD54" s="15"/>
+      <c r="AE54" s="15"/>
+      <c r="AF54" s="15"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
+      <c r="AJ54" s="15"/>
+      <c r="AK54" s="15"/>
+      <c r="AL54" s="3"/>
+      <c r="AM54" s="3"/>
+      <c r="AN54" s="7"/>
+      <c r="AO54" s="6"/>
+      <c r="AP54" s="1"/>
+      <c r="AQ54" s="5"/>
+      <c r="AR54" s="15"/>
+      <c r="AS54" s="15"/>
+      <c r="AT54" s="15"/>
+      <c r="AU54" s="15"/>
+      <c r="AV54" s="15"/>
+      <c r="AW54" s="15"/>
+      <c r="AX54" s="3"/>
+      <c r="AY54" s="15"/>
+      <c r="AZ54" s="15"/>
+      <c r="BA54" s="6"/>
+      <c r="BB54" s="1"/>
+      <c r="BC54" s="2"/>
+      <c r="BD54" s="12"/>
+      <c r="BE54" s="15"/>
+      <c r="BF54" s="1"/>
+      <c r="BG54" s="2"/>
+      <c r="BH54" s="15"/>
+      <c r="BI54" s="15"/>
+      <c r="BJ54" s="15"/>
+      <c r="BK54" s="2"/>
+      <c r="BL54" s="15"/>
+    </row>
+    <row r="55" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="V55" s="15"/>
+      <c r="W55" s="15"/>
+      <c r="X55" s="15"/>
+      <c r="Y55" s="15"/>
+      <c r="AA55" s="15"/>
+      <c r="AG55" s="15"/>
+      <c r="AH55" s="15"/>
+      <c r="AK55" s="15"/>
+      <c r="AS55" s="15"/>
+      <c r="AW55" s="15"/>
+      <c r="AY55" s="15"/>
+      <c r="BB55" s="15"/>
+      <c r="BE55" s="3"/>
+      <c r="BI55" s="15"/>
+      <c r="BK55" s="3"/>
+      <c r="BL55" s="3"/>
+    </row>
+    <row r="56" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>4</v>
       </c>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="1"/>
-      <c r="AC50" s="1"/>
-      <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-      <c r="AF50" s="1"/>
-      <c r="AG50" s="1"/>
-      <c r="AH50" s="1"/>
-      <c r="AI50" s="1"/>
-      <c r="AJ50" s="1"/>
-      <c r="AK50" s="1"/>
-      <c r="AL50" s="1"/>
-      <c r="AM50" s="1"/>
-      <c r="AN50" s="1"/>
-      <c r="AU50" s="1"/>
-      <c r="AV50" s="1"/>
-      <c r="AW50" s="1"/>
-      <c r="AX50" s="1"/>
-      <c r="AY50" s="1"/>
-      <c r="AZ50" s="1"/>
-      <c r="BC50" s="15"/>
-      <c r="BI50" s="1"/>
-      <c r="BJ50" s="1"/>
-    </row>
-    <row r="51" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="7"/>
-      <c r="N51" s="12"/>
-      <c r="P51" s="7"/>
-      <c r="R51" s="12"/>
-      <c r="T51" s="7"/>
-      <c r="V51" s="12"/>
-      <c r="X51" s="7"/>
-      <c r="AB51" s="12"/>
-      <c r="AN51" s="7"/>
-      <c r="AT51" s="12"/>
-      <c r="AZ51" s="7"/>
-      <c r="BB51" s="12"/>
-      <c r="BC51" s="5"/>
-      <c r="BD51" s="7"/>
-      <c r="BH51" s="12"/>
-      <c r="BJ51" s="7"/>
-    </row>
-    <row r="52" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="6"/>
-      <c r="F52" s="4"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="4"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="4"/>
-      <c r="T52" s="12"/>
-      <c r="U52" s="6"/>
-      <c r="V52" s="4"/>
-      <c r="X52" s="12"/>
-      <c r="Y52" s="6"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="4"/>
-      <c r="AN52" s="12"/>
-      <c r="AO52" s="6"/>
-      <c r="AP52" s="1"/>
-      <c r="AQ52" s="1"/>
-      <c r="AR52" s="1"/>
-      <c r="AS52" s="1"/>
-      <c r="AT52" s="4"/>
-      <c r="AZ52" s="12"/>
-      <c r="BA52" s="6"/>
-      <c r="BB52" s="4"/>
-      <c r="BD52" s="12"/>
-      <c r="BE52" s="6"/>
-      <c r="BF52" s="1"/>
-      <c r="BG52" s="1"/>
-      <c r="BH52" s="4"/>
-      <c r="BJ52" s="12"/>
-      <c r="BK52" s="6"/>
-      <c r="BL52" s="1"/>
-    </row>
-    <row r="53" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="BA53" s="15"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+      <c r="AL56" s="1"/>
+      <c r="AM56" s="1"/>
+      <c r="AN56" s="1"/>
+      <c r="AU56" s="1"/>
+      <c r="AV56" s="1"/>
+      <c r="AW56" s="1"/>
+      <c r="AX56" s="1"/>
+      <c r="AY56" s="1"/>
+      <c r="AZ56" s="1"/>
+      <c r="BC56" s="15"/>
+      <c r="BI56" s="1"/>
+      <c r="BJ56" s="1"/>
+    </row>
+    <row r="57" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="7"/>
+      <c r="N57" s="12"/>
+      <c r="P57" s="7"/>
+      <c r="R57" s="12"/>
+      <c r="T57" s="7"/>
+      <c r="V57" s="12"/>
+      <c r="X57" s="7"/>
+      <c r="AB57" s="12"/>
+      <c r="AN57" s="7"/>
+      <c r="AT57" s="12"/>
+      <c r="AZ57" s="7"/>
+      <c r="BB57" s="12"/>
+      <c r="BC57" s="5"/>
+      <c r="BD57" s="7"/>
+      <c r="BH57" s="12"/>
+      <c r="BJ57" s="7"/>
+    </row>
+    <row r="58" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="6"/>
+      <c r="F58" s="4"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="4"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="4"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="4"/>
+      <c r="X58" s="12"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="4"/>
+      <c r="AN58" s="12"/>
+      <c r="AO58" s="6"/>
+      <c r="AP58" s="1"/>
+      <c r="AQ58" s="1"/>
+      <c r="AR58" s="1"/>
+      <c r="AS58" s="1"/>
+      <c r="AT58" s="4"/>
+      <c r="AZ58" s="12"/>
+      <c r="BA58" s="6"/>
+      <c r="BB58" s="4"/>
+      <c r="BD58" s="12"/>
+      <c r="BE58" s="6"/>
+      <c r="BF58" s="1"/>
+      <c r="BG58" s="1"/>
+      <c r="BH58" s="4"/>
+      <c r="BJ58" s="12"/>
+      <c r="BK58" s="6"/>
+      <c r="BL58" s="1"/>
+    </row>
+    <row r="59" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="BA59" s="15"/>
+    </row>
+    <row r="60" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="L60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+      <c r="AV60" s="1"/>
+      <c r="AW60" s="1"/>
+      <c r="AZ60" s="1"/>
+      <c r="BA60" s="1"/>
+      <c r="BH60" s="1"/>
+    </row>
+    <row r="61" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="10"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="7"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="7"/>
+      <c r="L61" s="10"/>
+      <c r="N61" s="5"/>
+      <c r="P61" s="2"/>
+      <c r="R61" s="5"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="10"/>
+      <c r="W61" s="12"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="7"/>
+      <c r="AA61" s="12"/>
+      <c r="AC61" s="7"/>
+      <c r="AE61" s="12"/>
+      <c r="AF61" s="10"/>
+      <c r="AG61" s="13"/>
+      <c r="AH61" s="10"/>
+      <c r="AI61" s="13"/>
+      <c r="AJ61" s="10"/>
+      <c r="AK61" s="13"/>
+      <c r="AL61" s="10"/>
+      <c r="AM61" s="13"/>
+      <c r="AN61" s="10"/>
+      <c r="AO61" s="13"/>
+      <c r="AQ61" s="7"/>
+      <c r="AS61" s="12"/>
+      <c r="AT61" s="10"/>
+      <c r="AU61" s="13"/>
+      <c r="AW61" s="7"/>
+      <c r="AY61" s="12"/>
+      <c r="BA61" s="7"/>
+      <c r="BB61" s="13"/>
+      <c r="BC61" s="10"/>
+      <c r="BE61" s="12"/>
+      <c r="BF61" s="10"/>
+      <c r="BG61" s="13"/>
+      <c r="BH61" s="10"/>
+      <c r="BI61" s="13"/>
+      <c r="BJ61" s="10"/>
+      <c r="BK61" s="13"/>
+      <c r="BL61" s="5"/>
+    </row>
+    <row r="62" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="13"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="12"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="9"/>
+      <c r="P62" s="6"/>
+      <c r="R62" s="2"/>
+      <c r="T62" s="2"/>
+      <c r="U62" s="2"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="4"/>
+      <c r="Y62" s="12"/>
+      <c r="Z62" s="6"/>
+      <c r="AA62" s="4"/>
+      <c r="AC62" s="12"/>
+      <c r="AD62" s="6"/>
+      <c r="AE62" s="4"/>
+      <c r="AF62" s="13"/>
+      <c r="AG62" s="9"/>
+      <c r="AH62" s="13"/>
+      <c r="AI62" s="9"/>
+      <c r="AJ62" s="13"/>
+      <c r="AK62" s="9"/>
+      <c r="AL62" s="13"/>
+      <c r="AM62" s="9"/>
+      <c r="AN62" s="13"/>
+      <c r="AO62" s="9"/>
+      <c r="AQ62" s="12"/>
+      <c r="AR62" s="6"/>
+      <c r="AS62" s="4"/>
+      <c r="AT62" s="13"/>
+      <c r="AU62" s="9"/>
+      <c r="AW62" s="12"/>
+      <c r="AX62" s="6"/>
+      <c r="AY62" s="4"/>
+      <c r="BA62" s="12"/>
+      <c r="BB62" s="9"/>
+      <c r="BC62" s="13"/>
+      <c r="BE62" s="4"/>
+      <c r="BF62" s="13"/>
+      <c r="BG62" s="9"/>
+      <c r="BH62" s="13"/>
+      <c r="BI62" s="9"/>
+      <c r="BJ62" s="13"/>
+      <c r="BK62" s="9"/>
+    </row>
+    <row r="63" spans="1:64" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="AM63" s="3"/>
+      <c r="BB63" s="3"/>
+      <c r="BD63" s="3"/>
+      <c r="BG63" s="3"/>
+      <c r="BK63" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="BI45:BJ45"/>
-    <mergeCell ref="BK45:BL45"/>
-    <mergeCell ref="AY45:AZ45"/>
-    <mergeCell ref="BA45:BB45"/>
-    <mergeCell ref="BC45:BD45"/>
-    <mergeCell ref="BE45:BF45"/>
-    <mergeCell ref="BG45:BH45"/>
-    <mergeCell ref="AO45:AP45"/>
-    <mergeCell ref="AQ45:AR45"/>
-    <mergeCell ref="AS45:AT45"/>
-    <mergeCell ref="AU45:AV45"/>
-    <mergeCell ref="AW45:AX45"/>
-    <mergeCell ref="AE45:AF45"/>
-    <mergeCell ref="AG45:AH45"/>
-    <mergeCell ref="AI45:AJ45"/>
-    <mergeCell ref="AK45:AL45"/>
-    <mergeCell ref="AM45:AN45"/>
-    <mergeCell ref="A44:BL44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:X45"/>
-    <mergeCell ref="Y45:Z45"/>
-    <mergeCell ref="AA45:AB45"/>
-    <mergeCell ref="AC45:AD45"/>
+    <mergeCell ref="BI51:BJ51"/>
+    <mergeCell ref="BK51:BL51"/>
+    <mergeCell ref="AY51:AZ51"/>
+    <mergeCell ref="BA51:BB51"/>
+    <mergeCell ref="BC51:BD51"/>
+    <mergeCell ref="BE51:BF51"/>
+    <mergeCell ref="BG51:BH51"/>
+    <mergeCell ref="AO51:AP51"/>
+    <mergeCell ref="AQ51:AR51"/>
+    <mergeCell ref="AS51:AT51"/>
+    <mergeCell ref="AU51:AV51"/>
+    <mergeCell ref="AW51:AX51"/>
+    <mergeCell ref="AE51:AF51"/>
+    <mergeCell ref="AG51:AH51"/>
+    <mergeCell ref="AI51:AJ51"/>
+    <mergeCell ref="AK51:AL51"/>
+    <mergeCell ref="AM51:AN51"/>
+    <mergeCell ref="A50:BL50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="O51:P51"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="W51:X51"/>
+    <mergeCell ref="Y51:Z51"/>
+    <mergeCell ref="AA51:AB51"/>
+    <mergeCell ref="AC51:AD51"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>

</xml_diff>